<commit_message>
Added titanic solution, updated training schedule
</commit_message>
<xml_diff>
--- a/training schedule.xlsx
+++ b/training schedule.xlsx
@@ -5,37 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sus85\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\CV Training Guy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2376" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7670"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
   <si>
     <t>Supervisor</t>
   </si>
@@ -191,24 +181,75 @@
   </si>
   <si>
     <t>Unit 9 - Morpholy</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>Skimmed briefly, quite familiar</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t>Knowledge Before</t>
+  </si>
+  <si>
+    <t>Usefulness</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>4.5-5.5</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Graph exercise is great but does not look into the content of the commits which can be helpful</t>
+  </si>
+  <si>
+    <t>IMO can replace the pandas exercises, much more practical and concrete and made me look for various pandas tricks</t>
+  </si>
+  <si>
+    <t>5.5-6.5,12.5</t>
+  </si>
+  <si>
+    <t>7.5-12.5</t>
+  </si>
+  <si>
+    <t>6.5-12.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -216,7 +257,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -224,7 +265,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -232,14 +273,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -275,7 +316,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -359,6 +400,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -370,7 +422,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,10 +474,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - הדגשה1" xfId="3" builtinId="30"/>
@@ -435,7 +494,101 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="הדגשה1" xfId="2" builtinId="29"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FFFF66CC"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FFFF66CC"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -813,22 +966,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.25" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.9140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.25" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>27</v>
       </c>
@@ -841,9 +1000,23 @@
       <c r="D1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="25"/>
-    </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
@@ -853,78 +1026,150 @@
       </c>
       <c r="C2" s="20">
         <f>SUM(C3:C8)</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="D2" s="20"/>
-      <c r="E2"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
       <c r="D3" s="4"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
       <c r="D4" s="4"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4</v>
+      </c>
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <v>1.5</v>
+      </c>
       <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="24"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4">
+        <v>0.5</v>
+      </c>
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4">
+        <v>3.5</v>
+      </c>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -935,16 +1180,14 @@
       <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="21"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" s="17" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" s="17" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>34</v>
       </c>
@@ -957,11 +1200,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="16"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
@@ -972,9 +1217,9 @@
       <c r="D11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -986,7 +1231,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -998,7 +1243,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -1010,7 +1255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
@@ -1022,7 +1267,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
@@ -1034,7 +1279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
@@ -1046,7 +1291,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -1058,34 +1303,37 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="16">
         <f>SUM(B21,B29,B30)</f>
-        <v>29</v>
+        <v>23.5</v>
       </c>
       <c r="C20" s="16">
         <f>SUM(C21,C29,C30)</f>
         <v>0</v>
       </c>
       <c r="D20" s="16"/>
-      <c r="E20"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="2"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="6">
         <f>SUM(B22:B28)</f>
-        <v>23.5</v>
+        <v>18</v>
       </c>
       <c r="C21" s="6">
         <f>SUM(C22:C28)</f>
@@ -1093,7 +1341,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1105,79 +1353,79 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="4">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="4">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="4">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>43</v>
       </c>
@@ -1189,8 +1437,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="14">
@@ -1201,13 +1449,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="21"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>29</v>
       </c>
@@ -1221,7 +1469,7 @@
       </c>
       <c r="D32" s="16"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>30</v>
       </c>
@@ -1235,7 +1483,7 @@
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>12</v>
       </c>
@@ -1247,7 +1495,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>13</v>
       </c>
@@ -1259,7 +1507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
@@ -1271,7 +1519,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -1283,7 +1531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
@@ -1295,7 +1543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>17</v>
       </c>
@@ -1307,7 +1555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>31</v>
       </c>
@@ -1320,7 +1568,7 @@
       </c>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
@@ -1330,7 +1578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>19</v>
       </c>
@@ -1340,7 +1588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>20</v>
       </c>
@@ -1350,7 +1598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>32</v>
       </c>
@@ -1360,13 +1608,13 @@
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="21"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>1</v>
       </c>
@@ -1377,55 +1625,154 @@
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="12">
         <v>0.5</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="12">
+        <v>0.5</v>
+      </c>
       <c r="D47" s="12"/>
-    </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="E47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="2">
+        <v>2</v>
+      </c>
+      <c r="G47" s="2">
+        <v>4</v>
+      </c>
+      <c r="I47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="F48" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="12">
+        <v>0</v>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="F49" s="2">
+        <v>3</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D41">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>"Hadar and Yaniv"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1 D1:D1048576">
+  <conditionalFormatting sqref="D1:D47 D50:D1048576 E1:I2">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>"yoni and david"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+      <formula>"yoni"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+      <formula>"hadar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+      <formula>"david"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
+      <formula>"itay"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
+      <formula>"yaniv"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"yoni and david"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+      <formula>"yoni"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"hadar"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"david"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+      <formula>"itay"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+      <formula>"yaniv"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"yoni and david"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"yoni"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"hadar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"david"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"itay"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"yaniv"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>